<commit_message>
e13d and 13v update
</commit_message>
<xml_diff>
--- a/sample_status.xlsx
+++ b/sample_status.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zabdi/Documents/GitHub/fellowship-of-the-growth-rings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{238FD149-F0AC-D648-8752-BD7585FB59A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08568BA4-CF54-894A-B63B-F2978201B790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="1060" windowWidth="28040" windowHeight="16940" activeTab="1" xr2:uid="{9440439D-72F5-B441-976E-5500384619B7}"/>
+    <workbookView xWindow="760" yWindow="1060" windowWidth="28040" windowHeight="16940" activeTab="3" xr2:uid="{9440439D-72F5-B441-976E-5500384619B7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="E13A" sheetId="1" r:id="rId1"/>
+    <sheet name="E13C" sheetId="2" r:id="rId2"/>
+    <sheet name="E13D" sheetId="3" r:id="rId3"/>
+    <sheet name="E13V" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="31">
   <si>
     <t>SITE</t>
   </si>
@@ -118,6 +119,21 @@
   <si>
     <t>broken</t>
   </si>
+  <si>
+    <t>destroyed</t>
+  </si>
+  <si>
+    <t>Worked</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
 </sst>
 </file>
 
@@ -126,7 +142,7 @@
   <numFmts count="1">
     <numFmt numFmtId="170" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -141,6 +157,46 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -150,7 +206,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -158,11 +214,253 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -182,9 +480,87 @@
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="8">
     <dxf>
@@ -600,8 +976,8 @@
   <dimension ref="A1:G569"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E38" sqref="E38"/>
+      <pane ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2328,8 +2704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1B8BA3A-B3B9-D349-9807-AF47BAC6C8D8}">
   <dimension ref="A1:F206"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2661,7 +3037,7 @@
         <v>3</v>
       </c>
       <c r="E22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F22" s="1">
         <v>0</v>
@@ -2719,7 +3095,7 @@
         <v>3</v>
       </c>
       <c r="E26" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F26" s="1">
         <v>0</v>
@@ -2733,7 +3109,7 @@
         <v>4</v>
       </c>
       <c r="E27" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F27" s="1">
         <v>0</v>
@@ -2761,7 +3137,7 @@
         <v>6</v>
       </c>
       <c r="E29" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F29" s="1">
         <v>0</v>
@@ -2775,7 +3151,7 @@
         <v>7</v>
       </c>
       <c r="E30" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F30" s="1">
         <v>0</v>
@@ -2819,7 +3195,7 @@
         <v>2</v>
       </c>
       <c r="E33" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F33" s="1">
         <v>0</v>
@@ -2879,7 +3255,7 @@
         <v>2</v>
       </c>
       <c r="E37" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F37" s="1">
         <v>0</v>
@@ -2893,7 +3269,7 @@
         <v>3</v>
       </c>
       <c r="E38" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F38" s="1">
         <v>0</v>
@@ -2907,7 +3283,7 @@
         <v>4</v>
       </c>
       <c r="E39" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F39" s="1">
         <v>0</v>
@@ -2935,7 +3311,7 @@
         <v>6</v>
       </c>
       <c r="E41" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F41" s="1">
         <v>0</v>
@@ -2949,7 +3325,7 @@
         <v>7</v>
       </c>
       <c r="E42" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F42" s="1">
         <v>0</v>
@@ -2993,7 +3369,7 @@
         <v>2</v>
       </c>
       <c r="E45" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F45" s="1">
         <v>0</v>
@@ -3065,7 +3441,7 @@
         <v>3</v>
       </c>
       <c r="E50" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F50" s="1">
         <v>0</v>
@@ -3109,7 +3485,7 @@
         <v>2</v>
       </c>
       <c r="E53" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F53" s="1">
         <v>0</v>
@@ -3123,7 +3499,7 @@
         <v>3</v>
       </c>
       <c r="E54" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F54" s="1">
         <v>0</v>
@@ -3151,7 +3527,7 @@
         <v>5</v>
       </c>
       <c r="E56" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F56" s="1">
         <v>0</v>
@@ -3281,7 +3657,7 @@
         <v>2</v>
       </c>
       <c r="E65" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F65" s="1">
         <v>0</v>
@@ -3395,7 +3771,7 @@
         <v>4</v>
       </c>
       <c r="E73" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F73" s="1">
         <v>0</v>
@@ -3439,7 +3815,7 @@
         <v>2</v>
       </c>
       <c r="E76" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F76" s="1">
         <v>0</v>
@@ -3467,7 +3843,7 @@
         <v>4</v>
       </c>
       <c r="E78" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F78" s="1">
         <v>0</v>
@@ -3481,7 +3857,7 @@
         <v>5</v>
       </c>
       <c r="E79" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F79" s="1">
         <v>0</v>
@@ -3566,11 +3942,11 @@
       </c>
       <c r="E85" s="2">
         <f>SUM(E2:E84)</f>
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="F85" s="6">
         <f>(E85/E86)*100</f>
-        <v>66.265060240963862</v>
+        <v>91.566265060240966</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
@@ -3591,11 +3967,11 @@
       </c>
       <c r="E87" s="2">
         <f>E86-E85</f>
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="F87" s="6">
         <f>(E87/E86)*100</f>
-        <v>33.734939759036145</v>
+        <v>8.4337349397590362</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
@@ -3992,13 +4368,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C21D1B7D-9203-0A4B-BCF3-91ED701E39E0}">
-  <dimension ref="A1:F113"/>
+  <dimension ref="A1:G114"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="F113" sqref="F113"/>
+    <sheetView topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
@@ -4238,7 +4617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -4252,7 +4631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -4266,7 +4645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -4280,7 +4659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -4294,7 +4673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -4308,7 +4687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5" t="s">
@@ -4324,7 +4703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -4332,13 +4711,13 @@
         <v>2</v>
       </c>
       <c r="E23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F23" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -4346,13 +4725,13 @@
         <v>3</v>
       </c>
       <c r="E24" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F24" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -4366,21 +4745,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="1">
         <v>5</v>
       </c>
-      <c r="E26" s="1">
-        <v>0</v>
-      </c>
+      <c r="E26" s="1"/>
       <c r="F26" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -4394,7 +4774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5" t="s">
@@ -4410,7 +4790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -4418,13 +4798,13 @@
         <v>2</v>
       </c>
       <c r="E29" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F29" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -4438,7 +4818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -4446,13 +4826,13 @@
         <v>4</v>
       </c>
       <c r="E31" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F31" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -4460,7 +4840,7 @@
         <v>5</v>
       </c>
       <c r="E32" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F32" s="1">
         <v>0</v>
@@ -4675,21 +5055,19 @@
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
       <c r="D47" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E47" s="1">
-        <v>0</v>
-      </c>
-      <c r="F47" s="1">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F47" s="1"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="5"/>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
       <c r="D48" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E48" s="1">
         <v>1</v>
@@ -4701,11 +5079,9 @@
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="5"/>
       <c r="B49" s="5"/>
-      <c r="C49" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="C49" s="5"/>
       <c r="D49" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E49" s="1">
         <v>1</v>
@@ -4717,9 +5093,11 @@
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="5"/>
       <c r="B50" s="5"/>
-      <c r="C50" s="5"/>
+      <c r="C50" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="D50" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E50" s="1">
         <v>1</v>
@@ -4733,7 +5111,7 @@
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
       <c r="D51" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E51" s="1">
         <v>1</v>
@@ -4747,7 +5125,7 @@
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
       <c r="D52" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E52" s="1">
         <v>1</v>
@@ -4761,7 +5139,7 @@
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
       <c r="D53" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E53" s="1">
         <v>1</v>
@@ -4773,11 +5151,9 @@
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="5"/>
       <c r="B54" s="5"/>
-      <c r="C54" s="5" t="s">
-        <v>6</v>
-      </c>
+      <c r="C54" s="5"/>
       <c r="D54" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E54" s="1">
         <v>1</v>
@@ -4789,9 +5165,11 @@
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="5"/>
       <c r="B55" s="5"/>
-      <c r="C55" s="5"/>
+      <c r="C55" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="D55" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E55" s="1">
         <v>1</v>
@@ -4805,7 +5183,7 @@
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
       <c r="D56" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E56" s="1">
         <v>1</v>
@@ -4819,7 +5197,7 @@
       <c r="B57" s="5"/>
       <c r="C57" s="5"/>
       <c r="D57" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E57" s="1">
         <v>1</v>
@@ -4833,7 +5211,7 @@
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
       <c r="D58" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E58" s="1">
         <v>1</v>
@@ -4845,11 +5223,9 @@
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="5"/>
       <c r="B59" s="5"/>
-      <c r="C59" s="5" t="s">
-        <v>7</v>
-      </c>
+      <c r="C59" s="5"/>
       <c r="D59" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E59" s="1">
         <v>1</v>
@@ -4861,9 +5237,11 @@
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="5"/>
       <c r="B60" s="5"/>
-      <c r="C60" s="5"/>
+      <c r="C60" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="D60" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E60" s="1">
         <v>1</v>
@@ -4877,7 +5255,7 @@
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
       <c r="D61" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E61" s="1">
         <v>1</v>
@@ -4891,7 +5269,7 @@
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
       <c r="D62" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E62" s="1">
         <v>1</v>
@@ -4905,7 +5283,7 @@
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
       <c r="D63" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E63" s="1">
         <v>1</v>
@@ -4919,7 +5297,7 @@
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
       <c r="D64" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E64" s="1">
         <v>1</v>
@@ -4933,7 +5311,7 @@
       <c r="B65" s="5"/>
       <c r="C65" s="5"/>
       <c r="D65" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E65" s="1">
         <v>1</v>
@@ -4947,7 +5325,7 @@
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
       <c r="D66" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E66" s="1">
         <v>1</v>
@@ -4959,11 +5337,9 @@
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="5"/>
       <c r="B67" s="5"/>
-      <c r="C67" s="5" t="s">
+      <c r="C67" s="5"/>
+      <c r="D67" s="1">
         <v>8</v>
-      </c>
-      <c r="D67" s="1">
-        <v>1</v>
       </c>
       <c r="E67" s="1">
         <v>1</v>
@@ -4975,9 +5351,11 @@
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="5"/>
       <c r="B68" s="5"/>
-      <c r="C68" s="5"/>
+      <c r="C68" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="D68" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E68" s="1">
         <v>1</v>
@@ -4991,7 +5369,7 @@
       <c r="B69" s="5"/>
       <c r="C69" s="5"/>
       <c r="D69" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E69" s="1">
         <v>1</v>
@@ -5005,7 +5383,7 @@
       <c r="B70" s="5"/>
       <c r="C70" s="5"/>
       <c r="D70" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E70" s="1">
         <v>1</v>
@@ -5019,7 +5397,7 @@
       <c r="B71" s="5"/>
       <c r="C71" s="5"/>
       <c r="D71" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E71" s="1">
         <v>1</v>
@@ -5033,10 +5411,10 @@
       <c r="B72" s="5"/>
       <c r="C72" s="5"/>
       <c r="D72" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E72" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F72" s="1">
         <v>0</v>
@@ -5049,11 +5427,9 @@
         <v>9</v>
       </c>
       <c r="D73" s="1">
-        <v>1</v>
-      </c>
-      <c r="E73" s="1">
-        <v>1</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="E73" s="1"/>
       <c r="F73" s="1">
         <v>0</v>
       </c>
@@ -5063,7 +5439,7 @@
       <c r="B74" s="5"/>
       <c r="C74" s="5"/>
       <c r="D74" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E74" s="1">
         <v>1</v>
@@ -5077,7 +5453,7 @@
       <c r="B75" s="5"/>
       <c r="C75" s="5"/>
       <c r="D75" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E75" s="1">
         <v>1</v>
@@ -5091,7 +5467,7 @@
       <c r="B76" s="5"/>
       <c r="C76" s="5"/>
       <c r="D76" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E76" s="1">
         <v>1</v>
@@ -5102,14 +5478,10 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="5"/>
-      <c r="B77" s="5">
-        <v>3</v>
-      </c>
-      <c r="C77" s="5" t="s">
-        <v>11</v>
-      </c>
+      <c r="B77" s="5"/>
+      <c r="C77" s="5"/>
       <c r="D77" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E77" s="1">
         <v>1</v>
@@ -5120,10 +5492,14 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="5"/>
-      <c r="B78" s="5"/>
-      <c r="C78" s="5"/>
+      <c r="B78" s="5">
+        <v>3</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="D78" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E78" s="1">
         <v>1</v>
@@ -5137,10 +5513,10 @@
       <c r="B79" s="5"/>
       <c r="C79" s="5"/>
       <c r="D79" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E79" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F79" s="1">
         <v>0</v>
@@ -5151,7 +5527,7 @@
       <c r="B80" s="5"/>
       <c r="C80" s="5"/>
       <c r="D80" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E80" s="1">
         <v>1</v>
@@ -5163,11 +5539,9 @@
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="5"/>
       <c r="B81" s="5"/>
-      <c r="C81" s="5" t="s">
-        <v>6</v>
-      </c>
+      <c r="C81" s="5"/>
       <c r="D81" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E81" s="1">
         <v>1</v>
@@ -5179,12 +5553,14 @@
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="5"/>
       <c r="B82" s="5"/>
-      <c r="C82" s="5"/>
+      <c r="C82" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="D82" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E82" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F82" s="1">
         <v>0</v>
@@ -5195,7 +5571,7 @@
       <c r="B83" s="5"/>
       <c r="C83" s="5"/>
       <c r="D83" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E83" s="1">
         <v>0</v>
@@ -5209,7 +5585,7 @@
       <c r="B84" s="5"/>
       <c r="C84" s="5"/>
       <c r="D84" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E84" s="1">
         <v>0</v>
@@ -5223,10 +5599,10 @@
       <c r="B85" s="5"/>
       <c r="C85" s="5"/>
       <c r="D85" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E85" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F85" s="1">
         <v>0</v>
@@ -5237,10 +5613,10 @@
       <c r="B86" s="5"/>
       <c r="C86" s="5"/>
       <c r="D86" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E86" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F86" s="1">
         <v>0</v>
@@ -5251,7 +5627,7 @@
       <c r="B87" s="5"/>
       <c r="C87" s="5"/>
       <c r="D87" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E87" s="1">
         <v>0</v>
@@ -5265,7 +5641,7 @@
       <c r="B88" s="5"/>
       <c r="C88" s="5"/>
       <c r="D88" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E88" s="1">
         <v>0</v>
@@ -5279,10 +5655,10 @@
       <c r="B89" s="5"/>
       <c r="C89" s="5"/>
       <c r="D89" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E89" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F89" s="1">
         <v>0</v>
@@ -5291,11 +5667,9 @@
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" s="5"/>
       <c r="B90" s="5"/>
-      <c r="C90" s="5" t="s">
-        <v>7</v>
-      </c>
+      <c r="C90" s="5"/>
       <c r="D90" s="1">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E90" s="1">
         <v>1</v>
@@ -5307,12 +5681,14 @@
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="5"/>
       <c r="B91" s="5"/>
-      <c r="C91" s="5"/>
+      <c r="C91" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="D91" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E91" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F91" s="1">
         <v>0</v>
@@ -5323,10 +5699,10 @@
       <c r="B92" s="5"/>
       <c r="C92" s="5"/>
       <c r="D92" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E92" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F92" s="1">
         <v>0</v>
@@ -5337,7 +5713,7 @@
       <c r="B93" s="5"/>
       <c r="C93" s="5"/>
       <c r="D93" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E93" s="1">
         <v>0</v>
@@ -5351,10 +5727,10 @@
       <c r="B94" s="5"/>
       <c r="C94" s="5"/>
       <c r="D94" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E94" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F94" s="1">
         <v>0</v>
@@ -5365,7 +5741,7 @@
       <c r="B95" s="5"/>
       <c r="C95" s="5"/>
       <c r="D95" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E95" s="1">
         <v>0</v>
@@ -5379,10 +5755,10 @@
       <c r="B96" s="5"/>
       <c r="C96" s="5"/>
       <c r="D96" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E96" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F96" s="1">
         <v>0</v>
@@ -5391,11 +5767,9 @@
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" s="5"/>
       <c r="B97" s="5"/>
-      <c r="C97" s="5" t="s">
-        <v>8</v>
-      </c>
+      <c r="C97" s="5"/>
       <c r="D97" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E97" s="1">
         <v>1</v>
@@ -5407,12 +5781,14 @@
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" s="5"/>
       <c r="B98" s="5"/>
-      <c r="C98" s="5"/>
+      <c r="C98" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="D98" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E98" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F98" s="1">
         <v>0</v>
@@ -5423,10 +5799,10 @@
       <c r="B99" s="5"/>
       <c r="C99" s="5"/>
       <c r="D99" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E99" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F99" s="1">
         <v>0</v>
@@ -5437,10 +5813,10 @@
       <c r="B100" s="5"/>
       <c r="C100" s="5"/>
       <c r="D100" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E100" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F100" s="1">
         <v>0</v>
@@ -5451,10 +5827,10 @@
       <c r="B101" s="5"/>
       <c r="C101" s="5"/>
       <c r="D101" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E101" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F101" s="1">
         <v>0</v>
@@ -5463,11 +5839,9 @@
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" s="5"/>
       <c r="B102" s="5"/>
-      <c r="C102" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="C102" s="5"/>
       <c r="D102" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E102" s="1">
         <v>1</v>
@@ -5479,12 +5853,14 @@
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" s="5"/>
       <c r="B103" s="5"/>
-      <c r="C103" s="5"/>
+      <c r="C103" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="D103" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E103" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F103" s="1">
         <v>0</v>
@@ -5495,7 +5871,7 @@
       <c r="B104" s="5"/>
       <c r="C104" s="5"/>
       <c r="D104" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E104" s="1">
         <v>1</v>
@@ -5509,10 +5885,10 @@
       <c r="B105" s="5"/>
       <c r="C105" s="5"/>
       <c r="D105" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E105" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F105" s="1">
         <v>0</v>
@@ -5523,7 +5899,7 @@
       <c r="B106" s="5"/>
       <c r="C106" s="5"/>
       <c r="D106" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E106" s="1">
         <v>1</v>
@@ -5535,11 +5911,9 @@
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" s="5"/>
       <c r="B107" s="5"/>
-      <c r="C107" s="5" t="s">
-        <v>10</v>
-      </c>
+      <c r="C107" s="5"/>
       <c r="D107" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E107" s="1">
         <v>1</v>
@@ -5551,9 +5925,11 @@
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" s="5"/>
       <c r="B108" s="5"/>
-      <c r="C108" s="5"/>
+      <c r="C108" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="D108" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E108" s="1">
         <v>1</v>
@@ -5567,10 +5943,10 @@
       <c r="B109" s="5"/>
       <c r="C109" s="5"/>
       <c r="D109" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E109" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F109" s="1">
         <v>0</v>
@@ -5581,76 +5957,90 @@
       <c r="B110" s="5"/>
       <c r="C110" s="5"/>
       <c r="D110" s="1">
+        <v>3</v>
+      </c>
+      <c r="E110" s="1">
+        <v>1</v>
+      </c>
+      <c r="F110" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A111" s="5"/>
+      <c r="B111" s="5"/>
+      <c r="C111" s="5"/>
+      <c r="D111" s="1">
         <v>4</v>
       </c>
-      <c r="E110" s="1">
-        <v>1</v>
-      </c>
-      <c r="F110" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D111" t="s">
-        <v>21</v>
-      </c>
-      <c r="E111">
-        <f>SUM(E2:E110)</f>
-        <v>66</v>
-      </c>
-      <c r="F111">
-        <f>(E111/E113)*100</f>
-        <v>60.550458715596335</v>
+      <c r="E111" s="1">
+        <v>1</v>
+      </c>
+      <c r="F111" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D112" t="s">
+        <v>21</v>
+      </c>
+      <c r="E112">
+        <f>SUM(E2:E111)</f>
+        <v>77</v>
+      </c>
+      <c r="F112" s="7">
+        <f>(E112/E114)*100</f>
+        <v>71.296296296296291</v>
+      </c>
+    </row>
+    <row r="113" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D113" t="s">
         <v>20</v>
       </c>
-      <c r="E112">
-        <f>E113-E111</f>
-        <v>43</v>
-      </c>
-      <c r="F112">
-        <f>(E112/E113)*100</f>
-        <v>39.449541284403672</v>
-      </c>
-    </row>
-    <row r="113" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D113" t="s">
+      <c r="E113">
+        <f>E114-E112</f>
+        <v>31</v>
+      </c>
+      <c r="F113" s="7">
+        <f>(E113/E114)*100</f>
+        <v>28.703703703703702</v>
+      </c>
+    </row>
+    <row r="114" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D114" t="s">
         <v>19</v>
       </c>
-      <c r="E113">
-        <f>COUNT(E2:E110)</f>
-        <v>109</v>
+      <c r="E114">
+        <f>COUNT(E2:E111)</f>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="C102:C106"/>
-    <mergeCell ref="C73:C76"/>
-    <mergeCell ref="C77:C80"/>
-    <mergeCell ref="C81:C89"/>
-    <mergeCell ref="C90:C96"/>
-    <mergeCell ref="C97:C101"/>
+    <mergeCell ref="C108:C111"/>
+    <mergeCell ref="A2:A111"/>
+    <mergeCell ref="B78:B111"/>
+    <mergeCell ref="B42:B77"/>
+    <mergeCell ref="C46:C49"/>
+    <mergeCell ref="C50:C54"/>
+    <mergeCell ref="C55:C59"/>
+    <mergeCell ref="C60:C67"/>
+    <mergeCell ref="C68:C72"/>
+    <mergeCell ref="C73:C77"/>
+    <mergeCell ref="C78:C81"/>
+    <mergeCell ref="C82:C90"/>
+    <mergeCell ref="C91:C97"/>
+    <mergeCell ref="C98:C102"/>
+    <mergeCell ref="C103:C107"/>
     <mergeCell ref="B2:B41"/>
-    <mergeCell ref="A2:A110"/>
-    <mergeCell ref="B42:B76"/>
-    <mergeCell ref="B77:B110"/>
     <mergeCell ref="C2:C13"/>
     <mergeCell ref="C14:C21"/>
     <mergeCell ref="C22:C27"/>
     <mergeCell ref="C28:C33"/>
     <mergeCell ref="C34:C41"/>
     <mergeCell ref="C42:C45"/>
-    <mergeCell ref="C107:C110"/>
-    <mergeCell ref="C46:C48"/>
-    <mergeCell ref="C49:C53"/>
-    <mergeCell ref="C54:C58"/>
-    <mergeCell ref="C59:C66"/>
-    <mergeCell ref="C67:C72"/>
   </mergeCells>
-  <conditionalFormatting sqref="E2:E110">
+  <conditionalFormatting sqref="E2:E111">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
@@ -5664,10 +6054,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F22AE6DC-FDE9-0640-9C1E-562AC01C9AB6}">
-  <dimension ref="A1:F147"/>
+  <dimension ref="A1:G147"/>
   <sheetViews>
-    <sheetView topLeftCell="A116" workbookViewId="0">
-      <selection activeCell="F147" sqref="F147"/>
+    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="E94" sqref="E94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6346,7 +6736,7 @@
         <v>2</v>
       </c>
       <c r="E46" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F46" s="1">
         <v>0</v>
@@ -6360,7 +6750,7 @@
         <v>3</v>
       </c>
       <c r="E47" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F47" s="1">
         <v>0</v>
@@ -6380,7 +6770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="5"/>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
@@ -6388,13 +6778,13 @@
         <v>5</v>
       </c>
       <c r="E49" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F49" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="5"/>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
@@ -6408,7 +6798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="5"/>
       <c r="B51" s="5"/>
       <c r="C51" s="5" t="s">
@@ -6424,7 +6814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="5"/>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
@@ -6432,13 +6822,13 @@
         <v>2</v>
       </c>
       <c r="E52" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F52" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="5"/>
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
@@ -6446,13 +6836,13 @@
         <v>3</v>
       </c>
       <c r="E53" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F53" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="5"/>
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
@@ -6466,21 +6856,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="5"/>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
       <c r="D55" s="1">
         <v>5</v>
       </c>
-      <c r="E55" s="1">
-        <v>0</v>
-      </c>
+      <c r="E55" s="1"/>
       <c r="F55" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G55" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="5"/>
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
@@ -6488,13 +6879,13 @@
         <v>6</v>
       </c>
       <c r="E56" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F56" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="5"/>
       <c r="B57" s="5"/>
       <c r="C57" s="5"/>
@@ -6502,13 +6893,13 @@
         <v>7</v>
       </c>
       <c r="E57" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F57" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="5"/>
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
@@ -6522,7 +6913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="5"/>
       <c r="B59" s="5"/>
       <c r="C59" s="5" t="s">
@@ -6538,7 +6929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="5"/>
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
@@ -6546,13 +6937,13 @@
         <v>2</v>
       </c>
       <c r="E60" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F60" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="5"/>
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
@@ -6560,13 +6951,13 @@
         <v>3</v>
       </c>
       <c r="E61" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F61" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="5"/>
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
@@ -6580,7 +6971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="5"/>
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
@@ -6588,13 +6979,13 @@
         <v>5</v>
       </c>
       <c r="E63" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F63" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="5"/>
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
@@ -6608,7 +6999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="5"/>
       <c r="B65" s="5"/>
       <c r="C65" s="5" t="s">
@@ -6624,21 +7015,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="5"/>
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
       <c r="D66" s="1">
         <v>2</v>
       </c>
-      <c r="E66" s="1">
-        <v>0</v>
-      </c>
+      <c r="E66" s="1"/>
       <c r="F66" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G66" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="5"/>
       <c r="B67" s="5"/>
       <c r="C67" s="5"/>
@@ -6652,7 +7044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="5"/>
       <c r="B68" s="5"/>
       <c r="C68" s="5"/>
@@ -6666,7 +7058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="5"/>
       <c r="B69" s="5"/>
       <c r="C69" s="5" t="s">
@@ -6682,7 +7074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="5"/>
       <c r="B70" s="5"/>
       <c r="C70" s="5"/>
@@ -6690,13 +7082,13 @@
         <v>2</v>
       </c>
       <c r="E70" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F70" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="5"/>
       <c r="B71" s="5"/>
       <c r="C71" s="5"/>
@@ -6704,13 +7096,13 @@
         <v>3</v>
       </c>
       <c r="E71" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F71" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="5"/>
       <c r="B72" s="5"/>
       <c r="C72" s="5"/>
@@ -6724,7 +7116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="5"/>
       <c r="B73" s="5"/>
       <c r="C73" s="5"/>
@@ -6732,13 +7124,13 @@
         <v>5</v>
       </c>
       <c r="E73" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F73" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" s="5"/>
       <c r="B74" s="5"/>
       <c r="C74" s="5"/>
@@ -6752,7 +7144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="5"/>
       <c r="B75" s="5"/>
       <c r="C75" s="5" t="s">
@@ -6768,7 +7160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="5"/>
       <c r="B76" s="5"/>
       <c r="C76" s="5"/>
@@ -6776,13 +7168,13 @@
         <v>2</v>
       </c>
       <c r="E76" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F76" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" s="5"/>
       <c r="B77" s="5"/>
       <c r="C77" s="5"/>
@@ -6796,7 +7188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="5"/>
       <c r="B78" s="5"/>
       <c r="C78" s="5"/>
@@ -6804,13 +7196,13 @@
         <v>4</v>
       </c>
       <c r="E78" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F78" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" s="5"/>
       <c r="B79" s="5"/>
       <c r="C79" s="5"/>
@@ -6818,13 +7210,13 @@
         <v>5</v>
       </c>
       <c r="E79" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F79" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" s="5"/>
       <c r="B80" s="5"/>
       <c r="C80" s="5"/>
@@ -6862,7 +7254,7 @@
         <v>2</v>
       </c>
       <c r="E82" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F82" s="1">
         <v>0</v>
@@ -6876,7 +7268,7 @@
         <v>3</v>
       </c>
       <c r="E83" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F83" s="1">
         <v>0</v>
@@ -6904,7 +7296,7 @@
         <v>5</v>
       </c>
       <c r="E85" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F85" s="1">
         <v>0</v>
@@ -6918,7 +7310,7 @@
         <v>6</v>
       </c>
       <c r="E86" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F86" s="1">
         <v>0</v>
@@ -6932,7 +7324,7 @@
         <v>7</v>
       </c>
       <c r="E87" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F87" s="1">
         <v>0</v>
@@ -6990,7 +7382,7 @@
         <v>3</v>
       </c>
       <c r="E91" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F91" s="1">
         <v>0</v>
@@ -7760,11 +8152,11 @@
       </c>
       <c r="E145">
         <f>SUM(E2:E144)</f>
-        <v>88</v>
+        <v>110</v>
       </c>
       <c r="F145">
         <f>(E145/E147)*100</f>
-        <v>61.53846153846154</v>
+        <v>78.01418439716312</v>
       </c>
     </row>
     <row r="146" spans="4:6" x14ac:dyDescent="0.2">
@@ -7773,11 +8165,11 @@
       </c>
       <c r="E146">
         <f>E147-E145</f>
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="F146">
         <f>(E146/E147)*100</f>
-        <v>38.461538461538467</v>
+        <v>21.98581560283688</v>
       </c>
     </row>
     <row r="147" spans="4:6" x14ac:dyDescent="0.2">
@@ -7786,7 +8178,7 @@
       </c>
       <c r="E147">
         <f>COUNT(E2:E144)</f>
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -7828,4 +8220,590 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F2057EC-805C-ED4B-B4A5-E261467E16E2}">
+  <dimension ref="A1:J143"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="28" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="9"/>
+      <c r="B1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="13"/>
+      <c r="F1" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="15"/>
+      <c r="H1" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="17"/>
+      <c r="J1" s="18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="27" x14ac:dyDescent="0.35">
+      <c r="A2" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="20">
+        <f>E13A!E112</f>
+        <v>93</v>
+      </c>
+      <c r="C2" s="21">
+        <f>(B2/B4)</f>
+        <v>0.84545454545454546</v>
+      </c>
+      <c r="D2" s="38">
+        <f>E13C!E85</f>
+        <v>76</v>
+      </c>
+      <c r="E2" s="22">
+        <f>D2/D4</f>
+        <v>0.91566265060240959</v>
+      </c>
+      <c r="F2" s="23">
+        <f>E13D!E112</f>
+        <v>77</v>
+      </c>
+      <c r="G2" s="21">
+        <f>F2/F4</f>
+        <v>0.71296296296296291</v>
+      </c>
+      <c r="H2" s="24">
+        <f>E13V!E145</f>
+        <v>110</v>
+      </c>
+      <c r="I2" s="21">
+        <f>H2/H4</f>
+        <v>0.78014184397163122</v>
+      </c>
+      <c r="J2" s="25">
+        <f>(B2+D2+F2+H2)</f>
+        <v>356</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="28" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="27">
+        <f>E13A!E113</f>
+        <v>17</v>
+      </c>
+      <c r="C3" s="28">
+        <f>B3/B4</f>
+        <v>0.15454545454545454</v>
+      </c>
+      <c r="D3" s="39">
+        <f>E13C!E87</f>
+        <v>7</v>
+      </c>
+      <c r="E3" s="29">
+        <f>D3/D4</f>
+        <v>8.4337349397590355E-2</v>
+      </c>
+      <c r="F3" s="30">
+        <f>E13D!E113</f>
+        <v>31</v>
+      </c>
+      <c r="G3" s="28">
+        <f>F3/F4</f>
+        <v>0.28703703703703703</v>
+      </c>
+      <c r="H3" s="31">
+        <f>E13V!E146</f>
+        <v>31</v>
+      </c>
+      <c r="I3" s="28">
+        <f>H3/H4</f>
+        <v>0.21985815602836881</v>
+      </c>
+      <c r="J3" s="25">
+        <f>B3+D3+F3+H3</f>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="28" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="32">
+        <f>E13A!E114</f>
+        <v>110</v>
+      </c>
+      <c r="C4" s="33"/>
+      <c r="D4" s="34">
+        <f>E13C!E86</f>
+        <v>83</v>
+      </c>
+      <c r="E4" s="35"/>
+      <c r="F4" s="36">
+        <f>E13D!E114</f>
+        <v>108</v>
+      </c>
+      <c r="G4" s="33"/>
+      <c r="H4" s="37">
+        <f>E13V!E147</f>
+        <v>141</v>
+      </c>
+      <c r="I4" s="33"/>
+      <c r="J4" s="18">
+        <f>B4+D4+F4+H4</f>
+        <v>442</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H5" s="8"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F6" s="8"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="8"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F8" s="8"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F9" s="8"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F10" s="8"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F11" s="8"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F12" s="8"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F13" s="8"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F14" s="8"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F15" s="8"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F16" s="8"/>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F17" s="8"/>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F18" s="8"/>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F19" s="8"/>
+    </row>
+    <row r="20" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F20" s="8"/>
+    </row>
+    <row r="21" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F21" s="8"/>
+    </row>
+    <row r="22" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F22" s="8"/>
+    </row>
+    <row r="23" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F23" s="8"/>
+    </row>
+    <row r="24" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F24" s="8"/>
+    </row>
+    <row r="25" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F25" s="8"/>
+    </row>
+    <row r="26" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F26" s="8"/>
+    </row>
+    <row r="27" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F27" s="8"/>
+    </row>
+    <row r="28" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F28" s="8"/>
+    </row>
+    <row r="29" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F29" s="8"/>
+    </row>
+    <row r="30" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F30" s="8"/>
+    </row>
+    <row r="31" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F31" s="8"/>
+    </row>
+    <row r="32" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F32" s="8"/>
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F33" s="8"/>
+    </row>
+    <row r="34" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F34" s="8"/>
+    </row>
+    <row r="35" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F35" s="8"/>
+    </row>
+    <row r="36" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F36" s="8"/>
+    </row>
+    <row r="37" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F37" s="8"/>
+    </row>
+    <row r="38" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F38" s="8"/>
+    </row>
+    <row r="39" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F39" s="8"/>
+    </row>
+    <row r="40" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F40" s="8"/>
+    </row>
+    <row r="41" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F41" s="8"/>
+    </row>
+    <row r="42" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F42" s="8"/>
+    </row>
+    <row r="43" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F43" s="8"/>
+    </row>
+    <row r="44" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F44" s="8"/>
+    </row>
+    <row r="45" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F45" s="8"/>
+    </row>
+    <row r="46" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F46" s="8"/>
+    </row>
+    <row r="47" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F47" s="8"/>
+    </row>
+    <row r="48" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F48" s="8"/>
+    </row>
+    <row r="49" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F49" s="8"/>
+    </row>
+    <row r="50" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F50" s="8"/>
+    </row>
+    <row r="51" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F51" s="8"/>
+    </row>
+    <row r="52" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F52" s="8"/>
+    </row>
+    <row r="53" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F53" s="8"/>
+    </row>
+    <row r="54" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F54" s="8"/>
+    </row>
+    <row r="55" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F55" s="8"/>
+    </row>
+    <row r="56" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F56" s="8"/>
+    </row>
+    <row r="57" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F57" s="8"/>
+    </row>
+    <row r="58" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F58" s="8"/>
+    </row>
+    <row r="59" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F59" s="8"/>
+    </row>
+    <row r="60" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F60" s="8"/>
+    </row>
+    <row r="61" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F61" s="8"/>
+    </row>
+    <row r="62" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F62" s="8"/>
+    </row>
+    <row r="63" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F63" s="8"/>
+    </row>
+    <row r="64" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F64" s="8"/>
+    </row>
+    <row r="65" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F65" s="8"/>
+    </row>
+    <row r="66" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F66" s="8"/>
+    </row>
+    <row r="67" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F67" s="8"/>
+    </row>
+    <row r="68" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F68" s="8"/>
+    </row>
+    <row r="69" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F69" s="8"/>
+    </row>
+    <row r="70" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F70" s="8"/>
+    </row>
+    <row r="71" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F71" s="8"/>
+    </row>
+    <row r="72" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F72" s="8"/>
+    </row>
+    <row r="73" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F73" s="8"/>
+    </row>
+    <row r="74" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F74" s="8"/>
+    </row>
+    <row r="75" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F75" s="8"/>
+    </row>
+    <row r="76" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F76" s="8"/>
+    </row>
+    <row r="77" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F77" s="8"/>
+    </row>
+    <row r="78" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F78" s="8"/>
+    </row>
+    <row r="79" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F79" s="8"/>
+    </row>
+    <row r="80" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F80" s="8"/>
+    </row>
+    <row r="81" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F81" s="8"/>
+    </row>
+    <row r="82" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F82" s="8"/>
+    </row>
+    <row r="83" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F83" s="8"/>
+    </row>
+    <row r="84" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F84" s="8"/>
+    </row>
+    <row r="85" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F85" s="8"/>
+    </row>
+    <row r="86" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F86" s="8"/>
+    </row>
+    <row r="87" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F87" s="8"/>
+    </row>
+    <row r="88" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F88" s="8"/>
+    </row>
+    <row r="89" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F89" s="8"/>
+    </row>
+    <row r="90" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F90" s="8"/>
+    </row>
+    <row r="91" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F91" s="8"/>
+    </row>
+    <row r="92" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F92" s="8"/>
+    </row>
+    <row r="93" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F93" s="8"/>
+    </row>
+    <row r="94" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F94" s="8"/>
+    </row>
+    <row r="95" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F95" s="8"/>
+    </row>
+    <row r="96" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F96" s="8"/>
+    </row>
+    <row r="97" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F97" s="8"/>
+    </row>
+    <row r="98" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F98" s="8"/>
+    </row>
+    <row r="99" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F99" s="8"/>
+    </row>
+    <row r="100" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F100" s="8"/>
+    </row>
+    <row r="101" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F101" s="8"/>
+    </row>
+    <row r="102" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F102" s="8"/>
+    </row>
+    <row r="103" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F103" s="8"/>
+    </row>
+    <row r="104" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F104" s="8"/>
+    </row>
+    <row r="105" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F105" s="8"/>
+    </row>
+    <row r="106" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F106" s="8"/>
+    </row>
+    <row r="107" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F107" s="8"/>
+    </row>
+    <row r="108" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F108" s="8"/>
+    </row>
+    <row r="109" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F109" s="8"/>
+    </row>
+    <row r="110" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F110" s="8"/>
+    </row>
+    <row r="111" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F111" s="8"/>
+    </row>
+    <row r="112" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F112" s="8"/>
+    </row>
+    <row r="113" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F113" s="8"/>
+    </row>
+    <row r="114" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F114" s="8"/>
+    </row>
+    <row r="115" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F115" s="8"/>
+    </row>
+    <row r="116" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F116" s="8"/>
+    </row>
+    <row r="117" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F117" s="8"/>
+    </row>
+    <row r="118" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F118" s="8"/>
+    </row>
+    <row r="119" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F119" s="8"/>
+    </row>
+    <row r="120" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F120" s="8"/>
+    </row>
+    <row r="121" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F121" s="8"/>
+    </row>
+    <row r="122" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F122" s="8"/>
+    </row>
+    <row r="123" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F123" s="8"/>
+    </row>
+    <row r="124" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F124" s="8"/>
+    </row>
+    <row r="125" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F125" s="8"/>
+    </row>
+    <row r="126" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F126" s="8"/>
+    </row>
+    <row r="127" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F127" s="8"/>
+    </row>
+    <row r="128" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F128" s="8"/>
+    </row>
+    <row r="129" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F129" s="8"/>
+    </row>
+    <row r="130" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F130" s="8"/>
+    </row>
+    <row r="131" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F131" s="8"/>
+    </row>
+    <row r="132" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F132" s="8"/>
+    </row>
+    <row r="133" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F133" s="8"/>
+    </row>
+    <row r="134" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F134" s="8"/>
+    </row>
+    <row r="135" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F135" s="8"/>
+    </row>
+    <row r="136" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F136" s="8"/>
+    </row>
+    <row r="137" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F137" s="8"/>
+    </row>
+    <row r="138" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F138" s="8"/>
+    </row>
+    <row r="139" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F139" s="8"/>
+    </row>
+    <row r="140" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F140" s="8"/>
+    </row>
+    <row r="141" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F141" s="8"/>
+    </row>
+    <row r="142" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F142" s="8"/>
+    </row>
+    <row r="143" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F143" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>